<commit_message>
Add capture screenshot functionality
</commit_message>
<xml_diff>
--- a/TestData/testData.xlsx
+++ b/TestData/testData.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13695" windowHeight="2430"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -21,7 +22,7 @@
     <t>shailendra@appypie.com</t>
   </si>
   <si>
-    <t>secure@web1</t>
+    <t>secure@web</t>
   </si>
 </sst>
 </file>
@@ -374,7 +375,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
create new testcase for appy store search app
</commit_message>
<xml_diff>
--- a/TestData/testData.xlsx
+++ b/TestData/testData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="homepagetestdata" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -17,12 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>shailendra@appypie.com</t>
   </si>
   <si>
     <t>secure@web1</t>
+  </si>
+  <si>
+    <t>appiumvv</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -161,7 +164,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink display="shailendra@appypie.com" ref="A1" r:id="rId1"/>
-    <hyperlink display="secure@web" ref="B1" r:id="rId2"/>
+    <hyperlink display="secure@web1" ref="B1" r:id="rId2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -180,7 +183,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -188,7 +191,13 @@
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>

<commit_message>
added new pages with new test cases
</commit_message>
<xml_diff>
--- a/TestData/testData.xlsx
+++ b/TestData/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>shailendra@appypiellp.com</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>appium</t>
+  </si>
+  <si>
+    <t>3f2825e0033f</t>
   </si>
 </sst>
 </file>
@@ -140,9 +143,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -161,6 +164,7 @@
         <v>1</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink display="shailendra@appypiellp.com" ref="A1" r:id="rId1"/>
@@ -181,10 +185,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -195,6 +199,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>